<commit_message>
Agregada comprobacion de stock
solo muestra los que tengan disponibilidad
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89F553CC-FE45-4253-9824-5A5088B1E055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B976AFF-EA21-4316-B4E9-77C4F412B501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -48,6 +48,9 @@
     <t>FileId</t>
   </si>
   <si>
+    <t>Disponible</t>
+  </si>
+  <si>
     <t>Lineas verdes</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
     <t>1ptmOVmy_3wl_b6_22pLmamHQFqFb_oaM</t>
   </si>
   <si>
+    <t>si</t>
+  </si>
+  <si>
     <t>Blancas lisas</t>
   </si>
   <si>
@@ -75,6 +81,9 @@
     <t>1puPqNKoVCVGiV1-1Uz410e8rzaG6dkjb</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>Rosa y brillo</t>
   </si>
   <si>
@@ -102,7 +111,7 @@
     <t>Baby Square</t>
   </si>
   <si>
-    <t>1pQLTtWbM4fdGTYrjIUC59KSxRbaG_0M</t>
+    <t>1pQLTtWbM4fdGTYrjIUC59KSxRbaG_0Mt</t>
   </si>
   <si>
     <t>Corazones en rosa</t>
@@ -142,6 +151,30 @@
   </si>
   <si>
     <t>1oyICyFOV5qv_v-zuQY5r6HyMyJGqrAao</t>
+  </si>
+  <si>
+    <t>Rojas lisas</t>
+  </si>
+  <si>
+    <t>1pzDoLFjsip8QmHuF-JXWVboxEP2hgIMT</t>
+  </si>
+  <si>
+    <t>Amarillas lisas</t>
+  </si>
+  <si>
+    <t>1q9-QKZpkwh2m_l_nQQVD06hhAfZQYbwp</t>
+  </si>
+  <si>
+    <t>Celestes lisas</t>
+  </si>
+  <si>
+    <t>1q9RblGY49d_lSqEIxVWEDMYoCOP0slEZ</t>
+  </si>
+  <si>
+    <t>Violetas lisas</t>
+  </si>
+  <si>
+    <t>1qNxa9t8YnRFxEF9ltpW_f1ORKZPO9CGC</t>
   </si>
 </sst>
 </file>
@@ -504,20 +537,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="88.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,13 +570,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>2000</v>
@@ -551,18 +588,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1500</v>
@@ -571,18 +611,21 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>2000</v>
@@ -591,18 +634,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>1800</v>
@@ -611,18 +657,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>2000</v>
@@ -631,18 +680,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>1800</v>
@@ -651,18 +703,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>1800</v>
@@ -671,18 +726,21 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>1800</v>
@@ -691,18 +749,21 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1800</v>
@@ -711,18 +772,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>1500</v>
@@ -731,18 +795,21 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1800</v>
@@ -751,18 +818,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>1800</v>
@@ -771,18 +841,21 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>1800</v>
@@ -791,18 +864,21 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>2300</v>
@@ -811,10 +887,105 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>1500</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>1500</v>
+      </c>
+      <c r="D18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19">
+        <v>1500</v>
+      </c>
+      <c r="D19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -826,6 +997,8 @@
     <hyperlink ref="F7" r:id="rId5" display="https://drive.google.com/file/d/1pZpCTqJFgLsVT0b8VadZEbmv0LSSraci/view?usp=sharing" xr:uid="{76DA9680-BE9B-4E41-9A27-EF0E2088C9A9}"/>
     <hyperlink ref="F11" r:id="rId6" display="https://drive.google.com/file/d/1pBwbXrxse1wgVcqbCeYCN8h7hcG3-eOH/view?usp=sharing" xr:uid="{6F266611-1D07-402A-8251-00172060ECD1}"/>
     <hyperlink ref="F14" r:id="rId7" display="https://drive.google.com/file/d/1p88x0IfsALQzccNOAILmb3F_ppBuvggB/view?usp=sharing" xr:uid="{57D96DC6-0741-47DB-A579-3CE16F9E470B}"/>
+    <hyperlink ref="F18" r:id="rId8" display="https://drive.google.com/file/d/1q9RblGY49d_lSqEIxVWEDMYoCOP0slEZ/view?usp=sharing" xr:uid="{945D8BD0-8D4D-4B58-89BA-F46926F20D54}"/>
+    <hyperlink ref="F16" r:id="rId9" display="https://drive.google.com/file/d/1pzDoLFjsip8QmHuF-JXWVboxEP2hgIMT/view?usp=sharing" xr:uid="{AE783594-09C3-41C4-B8D8-C86BF868FD0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>